<commit_message>
Removed a duplicate motif from list and renamed motifs as appropriate.
</commit_message>
<xml_diff>
--- a/promoter_analyses/Dp_core_motifs/Top_Dp_de_novo_50_50.xlsx
+++ b/promoter_analyses/Dp_core_motifs/Top_Dp_de_novo_50_50.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21020" yWindow="0" windowWidth="30780" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="28500" yWindow="0" windowWidth="22800" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -300,8 +301,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -331,7 +340,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -339,6 +348,10 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -346,9 +359,33 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -716,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -822,7 +859,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B15" si="0">B2+1</f>
+        <f>B2+1</f>
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -864,7 +901,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f>B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -906,7 +943,7 @@
         <v>38</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f>B4+1</f>
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -942,7 +979,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f>B5+1</f>
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -981,44 +1018,38 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f>B6+1</f>
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="E7">
-        <v>10.33</v>
+        <v>4.04</v>
       </c>
       <c r="F7">
-        <v>39.700000000000003</v>
+        <v>42</v>
       </c>
       <c r="G7">
-        <v>-10.299999999999997</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>23</v>
+        <v>-8</v>
+      </c>
+      <c r="H7" s="2">
+        <v>9.9999999999999998E-150</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="J7" s="1">
-        <v>6.2300000000000001E-2</v>
+        <v>2.0301E-2</v>
       </c>
       <c r="K7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7">
-        <v>5.4199999999999995E-4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1026,32 +1057,32 @@
         <v>38</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f>B7+1</f>
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E8">
-        <v>4.04</v>
+        <v>1.89</v>
       </c>
       <c r="F8">
-        <v>42</v>
+        <v>44.5</v>
       </c>
       <c r="G8">
-        <v>-8</v>
+        <v>-5.5</v>
       </c>
       <c r="H8" s="2">
-        <v>9.9999999999999998E-150</v>
+        <v>1E-73</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="J8" s="1">
-        <v>2.0301E-2</v>
+        <v>1.7791000000000001E-2</v>
       </c>
       <c r="K8" t="s">
         <v>28</v>
@@ -1059,80 +1090,80 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <f>B8+1</f>
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>1.89</v>
+        <v>16.59</v>
       </c>
       <c r="F9">
-        <v>44.5</v>
+        <v>47.5</v>
       </c>
       <c r="G9">
-        <v>-5.5</v>
+        <v>-2.5</v>
       </c>
       <c r="H9" s="2">
-        <v>1E-73</v>
+        <v>9.9999999999999991E-308</v>
       </c>
       <c r="I9" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="J9" s="1">
-        <v>1.7791000000000001E-2</v>
+        <v>8.3799999999999996E-9</v>
       </c>
       <c r="K9" t="s">
         <v>28</v>
       </c>
+      <c r="L9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9">
+        <v>8.9700000000000005E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f>B9+1</f>
         <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E10">
-        <v>16.59</v>
+        <v>3.19</v>
       </c>
       <c r="F10">
-        <v>47.5</v>
+        <v>50.1</v>
       </c>
       <c r="G10">
-        <v>-2.5</v>
+        <v>0.10000000000000142</v>
       </c>
       <c r="H10" s="2">
-        <v>9.9999999999999991E-308</v>
+        <v>1E-210</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="J10" s="1">
-        <v>8.3799999999999996E-9</v>
+        <v>0.13467999999999999</v>
       </c>
       <c r="K10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10">
-        <v>8.9700000000000005E-3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1140,273 +1171,167 @@
         <v>38</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f>B10+1</f>
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E11">
-        <v>3.19</v>
+        <v>5.35</v>
       </c>
       <c r="F11">
-        <v>50.1</v>
+        <v>54.9</v>
       </c>
       <c r="G11">
-        <v>0.10000000000000142</v>
+        <v>4.8999999999999986</v>
       </c>
       <c r="H11" s="2">
-        <v>1E-210</v>
+        <v>9.9999999999999993E-77</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="J11" s="1">
-        <v>0.13467999999999999</v>
+        <v>1.2393E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f>B11+1</f>
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E12">
-        <v>5.35</v>
+        <v>1.02</v>
       </c>
       <c r="F12">
-        <v>54.9</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="G12">
-        <v>4.8999999999999986</v>
+        <v>10.799999999999997</v>
       </c>
       <c r="H12" s="2">
-        <v>9.9999999999999993E-77</v>
+        <v>1E-87</v>
       </c>
       <c r="I12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="1">
-        <v>1.2393E-2</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="J12" s="1"/>
       <c r="K12" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f>B12+1</f>
         <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E13">
-        <v>1.02</v>
+        <v>0.62</v>
       </c>
       <c r="F13">
-        <v>65.900000000000006</v>
+        <v>62.4</v>
       </c>
       <c r="G13">
-        <v>10.799999999999997</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="H13" s="2">
-        <v>1E-87</v>
+        <v>9.9999999999999993E-105</v>
       </c>
       <c r="I13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.7746000000000001E-2</v>
+      </c>
       <c r="K13" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="L13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13">
+        <v>5.5099999999999995E-4</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f>B13+1</f>
         <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E14">
-        <v>0.62</v>
+        <v>4.75</v>
       </c>
       <c r="F14">
-        <v>62.4</v>
+        <v>58.2</v>
       </c>
       <c r="G14">
-        <v>12.399999999999999</v>
+        <f>F14-50</f>
+        <v>8.2000000000000028</v>
       </c>
       <c r="H14" s="2">
-        <v>9.9999999999999993E-105</v>
+        <v>9.9999999999999995E-21</v>
       </c>
       <c r="I14" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="J14" s="1">
-        <v>1.7746000000000001E-2</v>
+        <v>7.1779000000000005E-4</v>
       </c>
       <c r="K14" t="s">
         <v>28</v>
-      </c>
-      <c r="L14" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14">
-        <v>5.5099999999999995E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15">
-        <v>4.75</v>
-      </c>
-      <c r="F15">
-        <v>58.2</v>
-      </c>
-      <c r="G15">
-        <f>F15-50</f>
-        <v>8.2000000000000028</v>
-      </c>
-      <c r="H15" s="2">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="I15" t="s">
-        <v>69</v>
-      </c>
-      <c r="J15" s="1">
-        <v>7.1779000000000005E-4</v>
-      </c>
-      <c r="K15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17">
-        <v>27.9</v>
-      </c>
-      <c r="F17">
-        <v>23.7</v>
-      </c>
-      <c r="G17">
-        <v>-26.3</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="1">
-        <v>7.4780000000000004E-10</v>
-      </c>
-      <c r="K17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18">
-        <v>3.94</v>
-      </c>
-      <c r="F18">
-        <v>42.2</v>
-      </c>
-      <c r="G18">
-        <v>-7.7999999999999972</v>
-      </c>
-      <c r="H18" s="2">
-        <v>1.0000000000000001E-293</v>
-      </c>
-      <c r="I18" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0.10278</v>
-      </c>
-      <c r="K18" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:M17">
     <sortCondition ref="F2:F17"/>
   </sortState>
-  <conditionalFormatting sqref="J2:J13 J17:J18">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="J2:J12">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="J14">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1418,4 +1343,141 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>27.9</v>
+      </c>
+      <c r="F2">
+        <v>23.7</v>
+      </c>
+      <c r="G2">
+        <v>-26.3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="1">
+        <v>7.4780000000000004E-10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3">
+        <v>3.94</v>
+      </c>
+      <c r="F3">
+        <v>42.2</v>
+      </c>
+      <c r="G3">
+        <v>-7.7999999999999972</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.0000000000000001E-293</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.10278</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f>Sheet1!B6+1</f>
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>10.33</v>
+      </c>
+      <c r="F4">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="G4">
+        <v>-10.299999999999997</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1">
+        <v>6.2300000000000001E-2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4">
+        <v>5.4199999999999995E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added updated Dp core master list
</commit_message>
<xml_diff>
--- a/promoter_analyses/Dp_core_motifs/Top_Dp_de_novo_50_50.xlsx
+++ b/promoter_analyses/Dp_core_motifs/Top_Dp_de_novo_50_50.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28500" yWindow="0" windowWidth="22800" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="15900" yWindow="0" windowWidth="35400" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
   <si>
     <t>Category</t>
   </si>
@@ -245,6 +245,45 @@
   </si>
   <si>
     <t>extra2</t>
+  </si>
+  <si>
+    <t>Dpm_ID</t>
+  </si>
+  <si>
+    <t>Dpm1</t>
+  </si>
+  <si>
+    <t>Dpm2</t>
+  </si>
+  <si>
+    <t>Dpm3</t>
+  </si>
+  <si>
+    <t>Dpm4</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Dpm5</t>
+  </si>
+  <si>
+    <t>Dpm6</t>
+  </si>
+  <si>
+    <t>Dpm8</t>
+  </si>
+  <si>
+    <t>Dpm7</t>
+  </si>
+  <si>
+    <t>Dpm9</t>
+  </si>
+  <si>
+    <t>Dpm10</t>
+  </si>
+  <si>
+    <t>MTE (#9)/MA0139.1_CTCF (Jaspar)</t>
   </si>
 </sst>
 </file>
@@ -301,8 +340,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -340,7 +393,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -352,6 +405,13 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -363,9 +423,26 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -753,30 +830,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="26.5" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
-    <col min="9" max="9" width="40" customWidth="1"/>
-    <col min="10" max="10" width="28.83203125" customWidth="1"/>
-    <col min="11" max="11" width="17.5" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="23.33203125" customWidth="1"/>
+    <col min="2" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="26.5" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" customWidth="1"/>
+    <col min="12" max="12" width="17.5" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1">
+    <row r="1" spans="1:14" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -784,554 +861,583 @@
         <v>70</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <f>1</f>
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>63</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>6.52</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>23.7</v>
       </c>
-      <c r="G2">
-        <f>F2-50</f>
+      <c r="H2">
+        <f>G2-50</f>
         <v>-26.3</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>7.4780000000000004E-10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3">
-        <f>B2+1</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3">
-        <v>3.42</v>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
       <c r="F3">
-        <v>24.6</v>
+        <v>8.99</v>
       </c>
       <c r="G3">
-        <v>-25.4</v>
-      </c>
-      <c r="H3" s="2">
-        <v>9.9999999999999991E-187</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="1">
-        <v>5.7615999999999998E-8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
+        <v>36.5</v>
+      </c>
+      <c r="H3">
+        <v>-13.5</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.13580999999999999</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3">
-        <v>6.3400000000000001E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>1.9599999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4">
-        <f>B3+1</f>
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <v>1.22</v>
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
       </c>
       <c r="F4">
-        <v>24.7</v>
+        <v>16.59</v>
       </c>
       <c r="G4">
-        <v>-25.3</v>
-      </c>
-      <c r="H4" s="2">
-        <v>9.9999999999999997E-73</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.19761000000000001</v>
-      </c>
-      <c r="K4" t="s">
-        <v>15</v>
+        <v>47.5</v>
+      </c>
+      <c r="H4">
+        <v>-2.5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>9.9999999999999991E-308</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="1">
+        <v>8.3799999999999996E-9</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4">
-        <v>1.5900000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4">
+        <v>8.9700000000000005E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>38</v>
       </c>
       <c r="B5">
-        <f>B4+1</f>
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5">
-        <v>1.82</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
       </c>
       <c r="F5">
-        <v>35.700000000000003</v>
+        <v>3.19</v>
       </c>
       <c r="G5">
-        <v>-14.299999999999997</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1E-150</v>
-      </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.18973999999999999</v>
-      </c>
-      <c r="K5" t="s">
+        <v>50.1</v>
+      </c>
+      <c r="H5">
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1E-210</v>
+      </c>
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.13467999999999999</v>
+      </c>
+      <c r="L5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <f>B5+1</f>
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>8.99</v>
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
       </c>
       <c r="F6">
-        <v>36.5</v>
+        <v>3.42</v>
       </c>
       <c r="G6">
-        <v>-13.5</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.13580999999999999</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
+        <v>24.6</v>
+      </c>
+      <c r="H6">
+        <v>-25.4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>9.9999999999999991E-187</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5.7615999999999998E-8</v>
       </c>
       <c r="L6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6">
-        <v>1.9599999999999999E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6">
+        <v>6.3400000000000001E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>38</v>
       </c>
       <c r="B7">
-        <f>B6+1</f>
-        <v>6</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7">
-        <v>4.04</v>
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
       </c>
       <c r="F7">
-        <v>42</v>
+        <v>1.82</v>
       </c>
       <c r="G7">
-        <v>-8</v>
-      </c>
-      <c r="H7" s="2">
-        <v>9.9999999999999998E-150</v>
-      </c>
-      <c r="I7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" s="1">
-        <v>2.0301E-2</v>
-      </c>
-      <c r="K7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="H7">
+        <v>-14.299999999999997</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1E-150</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.18973999999999999</v>
+      </c>
+      <c r="L7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>38</v>
       </c>
       <c r="B8">
-        <f>B7+1</f>
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8">
+        <v>4.04</v>
+      </c>
+      <c r="G8">
         <v>42</v>
       </c>
-      <c r="D8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8">
-        <v>1.89</v>
-      </c>
-      <c r="F8">
-        <v>44.5</v>
-      </c>
-      <c r="G8">
-        <v>-5.5</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1E-73</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1.7791000000000001E-2</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="H8">
+        <v>-8</v>
+      </c>
+      <c r="I8" s="2">
+        <v>9.9999999999999998E-150</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2.0301E-2</v>
+      </c>
+      <c r="L8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <f>B8+1</f>
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9">
-        <v>16.59</v>
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
       </c>
       <c r="F9">
-        <v>47.5</v>
+        <v>0.62</v>
       </c>
       <c r="G9">
-        <v>-2.5</v>
-      </c>
-      <c r="H9" s="2">
-        <v>9.9999999999999991E-308</v>
-      </c>
-      <c r="I9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="1">
-        <v>8.3799999999999996E-9</v>
-      </c>
-      <c r="K9" t="s">
+        <v>62.4</v>
+      </c>
+      <c r="H9">
+        <v>12.399999999999999</v>
+      </c>
+      <c r="I9" s="2">
+        <v>9.9999999999999993E-105</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.7746000000000001E-2</v>
+      </c>
+      <c r="L9" t="s">
         <v>28</v>
       </c>
-      <c r="L9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9">
-        <v>8.9700000000000005E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="M9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9">
+        <v>5.5099999999999995E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B10">
-        <f>B9+1</f>
-        <v>9</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10">
-        <v>3.19</v>
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
       </c>
       <c r="F10">
-        <v>50.1</v>
+        <v>1.02</v>
       </c>
       <c r="G10">
-        <v>0.10000000000000142</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1E-210</v>
-      </c>
-      <c r="I10" t="s">
-        <v>50</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0.13467999999999999</v>
-      </c>
-      <c r="K10" t="s">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="H10">
+        <v>10.799999999999997</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1E-87</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>38</v>
       </c>
       <c r="B11">
-        <f>B10+1</f>
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>5.35</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>54.9</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>4.8999999999999986</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>9.9999999999999993E-77</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>1.2393E-2</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B12">
-        <f>B11+1</f>
-        <v>11</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12">
-        <v>1.02</v>
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
       </c>
       <c r="F12">
-        <v>65.900000000000006</v>
+        <v>1.89</v>
       </c>
       <c r="G12">
-        <v>10.799999999999997</v>
-      </c>
-      <c r="H12" s="2">
-        <v>1E-87</v>
-      </c>
-      <c r="I12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>44.5</v>
+      </c>
+      <c r="H12">
+        <v>-5.5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1E-73</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1.7791000000000001E-2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">
-        <f>B12+1</f>
-        <v>12</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13">
-        <v>0.62</v>
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
       </c>
       <c r="F13">
-        <v>62.4</v>
+        <v>1.22</v>
       </c>
       <c r="G13">
-        <v>12.399999999999999</v>
-      </c>
-      <c r="H13" s="2">
-        <v>9.9999999999999993E-105</v>
-      </c>
-      <c r="I13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="1">
-        <v>1.7746000000000001E-2</v>
-      </c>
-      <c r="K13" t="s">
-        <v>28</v>
+        <v>24.7</v>
+      </c>
+      <c r="H13">
+        <v>-25.3</v>
+      </c>
+      <c r="I13" s="2">
+        <v>9.9999999999999997E-73</v>
+      </c>
+      <c r="J13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.19761000000000001</v>
       </c>
       <c r="L13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M13">
-        <v>5.5099999999999995E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>15</v>
+      </c>
+      <c r="M13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13">
+        <v>1.5900000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>38</v>
       </c>
       <c r="B14">
-        <f>B13+1</f>
         <v>13</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>68</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>4.75</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>58.2</v>
       </c>
-      <c r="G14">
-        <f>F14-50</f>
+      <c r="H14">
+        <f>G14-50</f>
         <v>8.2000000000000028</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>69</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>7.1779000000000005E-4</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:M17">
-    <sortCondition ref="F2:F17"/>
+  <sortState ref="A2:O14">
+    <sortCondition ref="I2:I14"/>
   </sortState>
-  <conditionalFormatting sqref="J2:J12">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="K4:K14">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1347,14 +1453,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
+    <row r="1" spans="1:13" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>57</v>
@@ -1429,9 +1576,9 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <f>Sheet1!B6+1</f>
-        <v>6</v>
+      <c r="B4" t="e">
+        <f>Sheet1!#REF!+1</f>
+        <v>#REF!</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -1469,7 +1616,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Saved spreadsheet containing master list of de novo motifs.
</commit_message>
<xml_diff>
--- a/promoter_analyses/Dp_core_motifs/Top_Dp_de_novo_50_50.xlsx
+++ b/promoter_analyses/Dp_core_motifs/Top_Dp_de_novo_50_50.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="0" windowWidth="35400" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="24480" yWindow="6920" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -340,8 +340,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -393,7 +397,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -412,6 +416,8 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -430,29 +436,11 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -833,7 +821,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -902,38 +890,43 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="F2">
-        <v>6.52</v>
+        <v>8.99</v>
       </c>
       <c r="G2">
-        <v>23.7</v>
+        <v>36.5</v>
       </c>
       <c r="H2">
-        <f>G2-50</f>
-        <v>-26.3</v>
+        <v>-13.5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="K2" s="1">
-        <v>7.4780000000000004E-10</v>
+        <v>0.13580999999999999</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2">
+        <v>1.9599999999999999E-3</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -941,43 +934,43 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F3">
-        <v>8.99</v>
+        <v>1.22</v>
       </c>
       <c r="G3">
-        <v>36.5</v>
+        <v>24.7</v>
       </c>
       <c r="H3">
-        <v>-13.5</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
+        <v>-25.3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>9.9999999999999997E-73</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="K3" s="1">
-        <v>0.13580999999999999</v>
+        <v>0.19761000000000001</v>
       </c>
       <c r="L3" t="s">
         <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N3">
-        <v>1.9599999999999999E-3</v>
+        <v>1.5900000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -985,163 +978,164 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F4">
-        <v>16.59</v>
+        <v>6.52</v>
       </c>
       <c r="G4">
-        <v>47.5</v>
+        <v>23.7</v>
       </c>
       <c r="H4">
-        <v>-2.5</v>
-      </c>
-      <c r="I4" s="2">
-        <v>9.9999999999999991E-308</v>
+        <f>G4-50</f>
+        <v>-26.3</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="K4" s="1">
-        <v>8.3799999999999996E-9</v>
+        <v>7.4780000000000004E-10</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
       </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4">
-        <v>8.9700000000000005E-3</v>
-      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="F5">
-        <v>3.19</v>
+        <v>16.59</v>
       </c>
       <c r="G5">
-        <v>50.1</v>
+        <v>47.5</v>
       </c>
       <c r="H5">
-        <v>0.10000000000000142</v>
+        <v>-2.5</v>
       </c>
       <c r="I5" s="2">
-        <v>1E-210</v>
+        <v>9.9999999999999991E-308</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="K5" s="1">
-        <v>0.13467999999999999</v>
+        <v>8.3799999999999996E-9</v>
       </c>
       <c r="L5" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5">
+        <v>8.9700000000000005E-3</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F6">
-        <v>3.42</v>
+        <v>3.19</v>
       </c>
       <c r="G6">
-        <v>24.6</v>
+        <v>50.1</v>
       </c>
       <c r="H6">
-        <v>-25.4</v>
+        <v>0.10000000000000142</v>
       </c>
       <c r="I6" s="2">
-        <v>9.9999999999999991E-187</v>
+        <v>1E-210</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="K6" s="1">
-        <v>5.7615999999999998E-8</v>
+        <v>0.13467999999999999</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6">
-        <v>6.3400000000000001E-4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="F7">
-        <v>1.82</v>
+        <v>3.42</v>
       </c>
       <c r="G7">
-        <v>35.700000000000003</v>
+        <v>24.6</v>
       </c>
       <c r="H7">
-        <v>-14.299999999999997</v>
+        <v>-25.4</v>
       </c>
       <c r="I7" s="2">
-        <v>1E-150</v>
+        <v>9.9999999999999991E-187</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="K7" s="1">
-        <v>0.18973999999999999</v>
+        <v>5.7615999999999998E-8</v>
       </c>
       <c r="L7" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7">
+        <v>6.3400000000000001E-4</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1228,38 +1222,40 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="F10">
-        <v>1.02</v>
+        <v>5.35</v>
       </c>
       <c r="G10">
-        <v>65.900000000000006</v>
+        <v>54.9</v>
       </c>
       <c r="H10">
-        <v>10.799999999999997</v>
+        <v>4.8999999999999986</v>
       </c>
       <c r="I10" s="2">
-        <v>1E-87</v>
+        <v>9.9999999999999993E-77</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1.2393E-2</v>
+      </c>
       <c r="L10" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1267,34 +1263,34 @@
         <v>38</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F11">
-        <v>5.35</v>
+        <v>1.89</v>
       </c>
       <c r="G11">
-        <v>54.9</v>
+        <v>44.5</v>
       </c>
       <c r="H11">
-        <v>4.8999999999999986</v>
+        <v>-5.5</v>
       </c>
       <c r="I11" s="2">
-        <v>9.9999999999999993E-77</v>
+        <v>1E-73</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K11" s="1">
-        <v>1.2393E-2</v>
+        <v>1.7791000000000001E-2</v>
       </c>
       <c r="L11" t="s">
         <v>28</v>
@@ -1305,81 +1301,73 @@
         <v>38</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F12">
-        <v>1.89</v>
+        <v>1.82</v>
       </c>
       <c r="G12">
-        <v>44.5</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="H12">
-        <v>-5.5</v>
+        <v>-14.299999999999997</v>
       </c>
       <c r="I12" s="2">
-        <v>1E-73</v>
+        <v>1E-150</v>
       </c>
       <c r="J12" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K12" s="1">
-        <v>1.7791000000000001E-2</v>
+        <v>0.18973999999999999</v>
       </c>
       <c r="L12" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F13">
-        <v>1.22</v>
+        <v>1.02</v>
       </c>
       <c r="G13">
-        <v>24.7</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="H13">
-        <v>-25.3</v>
+        <v>10.799999999999997</v>
       </c>
       <c r="I13" s="2">
-        <v>9.9999999999999997E-73</v>
+        <v>1E-87</v>
       </c>
       <c r="J13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0.19761000000000001</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="K13" s="1"/>
       <c r="L13" t="s">
         <v>15</v>
-      </c>
-      <c r="M13" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13">
-        <v>1.5900000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1422,22 +1410,22 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:O14">
-    <sortCondition ref="I2:I14"/>
+  <sortState ref="A2:N14">
+    <sortCondition ref="C2:C14"/>
   </sortState>
   <conditionalFormatting sqref="K4:K14">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1456,7 +1444,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1616,7 +1604,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removed duplicate motifs from Dpm_core set and updated master list.
</commit_message>
<xml_diff>
--- a/promoter_analyses/Dp_core_motifs/Top_Dp_de_novo_50_50.xlsx
+++ b/promoter_analyses/Dp_core_motifs/Top_Dp_de_novo_50_50.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24480" yWindow="6920" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="30860" yWindow="6940" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
   <si>
     <t>Category</t>
   </si>
@@ -275,12 +275,6 @@
   </si>
   <si>
     <t>Dpm7</t>
-  </si>
-  <si>
-    <t>Dpm9</t>
-  </si>
-  <si>
-    <t>Dpm10</t>
   </si>
   <si>
     <t>MTE (#9)/MA0139.1_CTCF (Jaspar)</t>
@@ -340,8 +334,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -397,7 +397,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -418,6 +418,9 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -438,9 +441,92 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -821,7 +907,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -937,7 +1023,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
@@ -958,7 +1044,7 @@
         <v>9.9999999999999997E-73</v>
       </c>
       <c r="J3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K3" s="1">
         <v>0.19761000000000001</v>
@@ -1140,84 +1226,84 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F8">
-        <v>4.04</v>
+        <v>0.62</v>
       </c>
       <c r="G8">
-        <v>42</v>
+        <v>62.4</v>
       </c>
       <c r="H8">
-        <v>-8</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="I8" s="2">
-        <v>9.9999999999999998E-150</v>
+        <v>9.9999999999999993E-105</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="K8" s="1">
-        <v>2.0301E-2</v>
+        <v>1.7746000000000001E-2</v>
       </c>
       <c r="L8" t="s">
         <v>28</v>
+      </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8">
+        <v>5.5099999999999995E-4</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>84</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F9">
-        <v>0.62</v>
+        <v>1.89</v>
       </c>
       <c r="G9">
-        <v>62.4</v>
+        <v>44.5</v>
       </c>
       <c r="H9">
-        <v>12.399999999999999</v>
+        <v>-5.5</v>
       </c>
       <c r="I9" s="2">
-        <v>9.9999999999999993E-105</v>
+        <v>1E-73</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="K9" s="1">
-        <v>1.7746000000000001E-2</v>
+        <v>1.7791000000000001E-2</v>
       </c>
       <c r="L9" t="s">
         <v>28</v>
-      </c>
-      <c r="M9" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9">
-        <v>5.5099999999999995E-4</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1225,75 +1311,73 @@
         <v>38</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="F10">
-        <v>5.35</v>
+        <v>1.82</v>
       </c>
       <c r="G10">
-        <v>54.9</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="H10">
-        <v>4.8999999999999986</v>
+        <v>-14.299999999999997</v>
       </c>
       <c r="I10" s="2">
-        <v>9.9999999999999993E-77</v>
+        <v>1E-150</v>
       </c>
       <c r="J10" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="K10" s="1">
-        <v>1.2393E-2</v>
+        <v>0.18973999999999999</v>
       </c>
       <c r="L10" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="F11">
-        <v>1.89</v>
+        <v>1.02</v>
       </c>
       <c r="G11">
-        <v>44.5</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="H11">
-        <v>-5.5</v>
+        <v>10.799999999999997</v>
       </c>
       <c r="I11" s="2">
-        <v>1E-73</v>
+        <v>1E-87</v>
       </c>
       <c r="J11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" s="1">
-        <v>1.7791000000000001E-2</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="K11" s="1"/>
       <c r="L11" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1301,73 +1385,76 @@
         <v>38</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>80</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="F12">
-        <v>1.82</v>
+        <v>4.75</v>
       </c>
       <c r="G12">
-        <v>35.700000000000003</v>
+        <v>58.2</v>
       </c>
       <c r="H12">
-        <v>-14.299999999999997</v>
+        <f>G12-50</f>
+        <v>8.2000000000000028</v>
       </c>
       <c r="I12" s="2">
-        <v>1E-150</v>
+        <v>9.9999999999999995E-21</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="K12" s="1">
-        <v>0.18973999999999999</v>
+        <v>7.1779000000000005E-4</v>
       </c>
       <c r="L12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>80</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="F13">
-        <v>1.02</v>
+        <v>4.04</v>
       </c>
       <c r="G13">
-        <v>65.900000000000006</v>
+        <v>42</v>
       </c>
       <c r="H13">
-        <v>10.799999999999997</v>
+        <v>-8</v>
       </c>
       <c r="I13" s="2">
-        <v>1E-87</v>
+        <v>9.9999999999999998E-150</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2.0301E-2</v>
+      </c>
       <c r="L13" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1375,35 +1462,34 @@
         <v>38</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
         <v>80</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="F14">
-        <v>4.75</v>
+        <v>5.35</v>
       </c>
       <c r="G14">
-        <v>58.2</v>
+        <v>54.9</v>
       </c>
       <c r="H14">
-        <f>G14-50</f>
-        <v>8.2000000000000028</v>
+        <v>4.8999999999999986</v>
       </c>
       <c r="I14" s="2">
-        <v>9.9999999999999995E-21</v>
+        <v>9.9999999999999993E-77</v>
       </c>
       <c r="J14" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="K14" s="1">
-        <v>7.1779000000000005E-4</v>
+        <v>1.2393E-2</v>
       </c>
       <c r="L14" t="s">
         <v>28</v>
@@ -1413,20 +1499,30 @@
   <sortState ref="A2:N14">
     <sortCondition ref="C2:C14"/>
   </sortState>
-  <conditionalFormatting sqref="K4:K14">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="K4:K12">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
       <formula>0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1444,7 +1540,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A6" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1604,11 +1700,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>